<commit_message>
Fixed bug in writing rich strings
</commit_message>
<xml_diff>
--- a/gptables/examples/iris_gptable.xlsx
+++ b/gptables/examples/iris_gptable.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <r>
       <t>Mean</t>
@@ -33,6 +33,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -55,7 +56,10 @@
     <t>cm(2)</t>
   </si>
   <si>
-    <t>All(3)</t>
+    <t>Mean Sepal Length</t>
+  </si>
+  <si>
+    <t>Mean Sepal Width</t>
   </si>
   <si>
     <t>Setosa</t>
@@ -67,24 +71,6 @@
     <t>Virginica</t>
   </si>
   <si>
-    <t xml:space="preserve"> petal_length</t>
-  </si>
-  <si>
-    <t>Mean</t>
-  </si>
-  <si>
-    <t>Median</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> petal_width</t>
-  </si>
-  <si>
-    <t>Sepal Length</t>
-  </si>
-  <si>
-    <t>Sepal Width</t>
-  </si>
-  <si>
     <t>(Source: Office for Iris Statistics)</t>
   </si>
   <si>
@@ -92,9 +78,6 @@
   </si>
   <si>
     <t>(2: I've got 99 problems and taxonomy is one.)</t>
-  </si>
-  <si>
-    <t>(3: All species of the Iris genus.)</t>
   </si>
   <si>
     <t>(This note hath no reference.)</t>
@@ -480,234 +463,95 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:3">
       <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="5" t="s">
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="B6" s="6">
+        <v>5.005999999999999</v>
+      </c>
+      <c r="C6" s="6">
+        <v>3.418000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="1" t="s">
+      <c r="B7" s="6">
+        <v>5.936</v>
+      </c>
+      <c r="C7" s="6">
+        <v>2.77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B8" s="6">
+        <v>6.587999999999998</v>
+      </c>
+      <c r="C8" s="6">
+        <v>2.974</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="6">
-        <v>3.758666666666666</v>
-      </c>
-      <c r="D6" s="6">
-        <v>1.464</v>
-      </c>
-      <c r="E6" s="6">
-        <v>4.26</v>
-      </c>
-      <c r="F6" s="6">
-        <v>5.552</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="3" t="s">
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="6">
-        <v>4.35</v>
-      </c>
-      <c r="D7" s="6">
-        <v>1.5</v>
-      </c>
-      <c r="E7" s="6">
-        <v>4.35</v>
-      </c>
-      <c r="F7" s="6">
-        <v>5.55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1" t="s">
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="6">
-        <v>1.198666666666667</v>
-      </c>
-      <c r="D8" s="6">
-        <v>0.2439999999999999</v>
-      </c>
-      <c r="E8" s="6">
-        <v>1.326</v>
-      </c>
-      <c r="F8" s="6">
-        <v>2.026</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="6">
-        <v>1.3</v>
-      </c>
-      <c r="D9" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="E9" s="6">
-        <v>1.3</v>
-      </c>
-      <c r="F9" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="1" t="s">
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="6">
-        <v>5.843333333333334</v>
-      </c>
-      <c r="D10" s="6">
-        <v>5.005999999999999</v>
-      </c>
-      <c r="E10" s="6">
-        <v>5.936</v>
-      </c>
-      <c r="F10" s="6">
-        <v>6.587999999999998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="6">
-        <v>5.8</v>
-      </c>
-      <c r="D11" s="6">
-        <v>5</v>
-      </c>
-      <c r="E11" s="6">
-        <v>5.9</v>
-      </c>
-      <c r="F11" s="6">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="6">
-        <v>3.054</v>
-      </c>
-      <c r="D12" s="6">
-        <v>3.418000000000001</v>
-      </c>
-      <c r="E12" s="6">
-        <v>2.77</v>
-      </c>
-      <c r="F12" s="6">
-        <v>2.974</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="6">
-        <v>3</v>
-      </c>
-      <c r="D13" s="6">
-        <v>3.4</v>
-      </c>
-      <c r="E13" s="6">
-        <v>2.8</v>
-      </c>
-      <c r="F13" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="7" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>